<commit_message>
Remove prawns from prawns/shrimps
</commit_message>
<xml_diff>
--- a/data/Food_Footprints_SinglePage.xlsx
+++ b/data/Food_Footprints_SinglePage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD26D355-C14B-494C-B610-DC88386429CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466A3B41-4A0F-4032-BB46-119317601C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,18 +1314,12 @@
     <t>CRUSTACEAN* (SUB-TYP) (Prawns/Shrimps)</t>
   </si>
   <si>
-    <t>PRAWNS/SHRIMPS</t>
-  </si>
-  <si>
     <t>SHELLFISH FROZEN</t>
   </si>
   <si>
     <t>OCTOPUS (F)</t>
   </si>
   <si>
-    <t>PRAWNS/SHRIMPS (F)</t>
-  </si>
-  <si>
     <t>Typology</t>
   </si>
   <si>
@@ -1345,6 +1339,12 @@
   </si>
   <si>
     <t>CHILI</t>
+  </si>
+  <si>
+    <t>SHRIMPS (F)</t>
+  </si>
+  <si>
+    <t>SHRIMPS</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="C327" sqref="C327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,13 +1910,13 @@
   <sheetData>
     <row r="1" spans="1:24" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -3516,7 +3516,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -12898,7 +12898,7 @@
         <v>238</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D173" s="13">
         <v>2</v>
@@ -16272,7 +16272,7 @@
         <v>18</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D226" s="13">
         <v>1</v>
@@ -20610,7 +20610,7 @@
         <v>18</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D294" s="13">
         <v>2</v>
@@ -22398,7 +22398,7 @@
         <v>411</v>
       </c>
       <c r="C322" s="12" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="D322" s="13">
         <v>18</v>
@@ -22456,13 +22456,13 @@
     </row>
     <row r="323" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B323" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C323" s="12" t="s">
         <v>413</v>
-      </c>
-      <c r="B323" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C323" s="12" t="s">
-        <v>414</v>
       </c>
       <c r="D323" s="13">
         <v>1</v>
@@ -22520,13 +22520,13 @@
     </row>
     <row r="324" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B324" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C324" s="12" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="D324" s="13">
         <v>4</v>

</xml_diff>

<commit_message>
Add co2 and nutrient data filtered by known words
</commit_message>
<xml_diff>
--- a/data/Food_Footprints_SinglePage.xlsx
+++ b/data/Food_Footprints_SinglePage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466A3B41-4A0F-4032-BB46-119317601C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01C5E1-92AA-4FD4-8FD8-B9DF5D15A314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,9 +918,6 @@
     <t>COWPEA</t>
   </si>
   <si>
-    <t>GREEN BEAN (fresh)</t>
-  </si>
-  <si>
     <t>LENTIL</t>
   </si>
   <si>
@@ -933,9 +930,6 @@
     <t>LEGUMES NOT HEATED GREENHOUSE (green bean)</t>
   </si>
   <si>
-    <t>GREEN BEAN (fresh) (g)*</t>
-  </si>
-  <si>
     <t>MUSHROOM*</t>
   </si>
   <si>
@@ -1345,6 +1339,12 @@
   </si>
   <si>
     <t>SHRIMPS</t>
+  </si>
+  <si>
+    <t>GREEN BEAN fresh (g)*</t>
+  </si>
+  <si>
+    <t>GREEN BEAN fresh</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
-      <selection activeCell="C327" sqref="C327"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C207" sqref="C207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,13 +1910,13 @@
   <sheetData>
     <row r="1" spans="1:24" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -3516,7 +3516,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -12898,7 +12898,7 @@
         <v>238</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D173" s="13">
         <v>2</v>
@@ -15062,7 +15062,7 @@
         <v>18</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>280</v>
+        <v>422</v>
       </c>
       <c r="D207" s="13">
         <v>11</v>
@@ -15126,7 +15126,7 @@
         <v>18</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D208" s="13">
         <v>2</v>
@@ -15190,7 +15190,7 @@
         <v>18</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D209" s="13">
         <v>12</v>
@@ -15254,7 +15254,7 @@
         <v>18</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D210" s="13">
         <v>5</v>
@@ -15312,13 +15312,13 @@
     </row>
     <row r="211" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B211" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>285</v>
+        <v>421</v>
       </c>
       <c r="D211" s="13">
         <v>4</v>
@@ -15376,11 +15376,11 @@
     </row>
     <row r="212" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B212" s="11"/>
       <c r="C212" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D212" s="13">
         <v>6</v>
@@ -15438,13 +15438,13 @@
     </row>
     <row r="213" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B213" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D213" s="13">
         <v>13</v>
@@ -15502,13 +15502,13 @@
     </row>
     <row r="214" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B214" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C214" s="12" t="s">
         <v>287</v>
-      </c>
-      <c r="B214" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C214" s="12" t="s">
-        <v>289</v>
       </c>
       <c r="D214" s="13">
         <v>11</v>
@@ -15566,13 +15566,13 @@
     </row>
     <row r="215" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B215" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D215" s="13">
         <v>3</v>
@@ -15628,13 +15628,13 @@
     </row>
     <row r="216" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B216" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D216" s="13">
         <v>5</v>
@@ -15692,13 +15692,13 @@
     </row>
     <row r="217" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B217" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D217" s="13">
         <v>1</v>
@@ -15756,13 +15756,13 @@
     </row>
     <row r="218" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B218" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D218" s="13">
         <v>1</v>
@@ -15820,13 +15820,13 @@
     </row>
     <row r="219" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B219" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D219" s="13">
         <v>10</v>
@@ -15884,13 +15884,13 @@
     </row>
     <row r="220" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B220" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D220" s="13">
         <v>4</v>
@@ -15948,13 +15948,13 @@
     </row>
     <row r="221" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B221" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D221" s="13">
         <v>5</v>
@@ -16012,13 +16012,13 @@
     </row>
     <row r="222" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B222" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D222" s="13">
         <v>35</v>
@@ -16076,13 +16076,13 @@
     </row>
     <row r="223" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B223" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D223" s="13">
         <v>3</v>
@@ -16138,13 +16138,13 @@
     </row>
     <row r="224" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B224" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C224" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="B224" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C224" s="12" t="s">
-        <v>300</v>
       </c>
       <c r="D224" s="13">
         <v>1</v>
@@ -16202,13 +16202,13 @@
     </row>
     <row r="225" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B225" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D225" s="13">
         <v>2</v>
@@ -16266,13 +16266,13 @@
     </row>
     <row r="226" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B226" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D226" s="13">
         <v>1</v>
@@ -16330,13 +16330,13 @@
     </row>
     <row r="227" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B227" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D227" s="13">
         <v>1</v>
@@ -16394,13 +16394,13 @@
     </row>
     <row r="228" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B228" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D228" s="13">
         <v>35</v>
@@ -16458,13 +16458,13 @@
     </row>
     <row r="229" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B229" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C229" s="12" t="s">
         <v>304</v>
-      </c>
-      <c r="B229" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C229" s="12" t="s">
-        <v>306</v>
       </c>
       <c r="D229" s="13">
         <v>2</v>
@@ -16522,13 +16522,13 @@
     </row>
     <row r="230" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B230" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D230" s="13">
         <v>3</v>
@@ -16584,13 +16584,13 @@
     </row>
     <row r="231" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B231" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D231" s="13">
         <v>8</v>
@@ -16648,13 +16648,13 @@
     </row>
     <row r="232" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B232" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C232" s="12" t="s">
         <v>308</v>
-      </c>
-      <c r="B232" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C232" s="12" t="s">
-        <v>310</v>
       </c>
       <c r="D232" s="13">
         <v>4</v>
@@ -16712,13 +16712,13 @@
     </row>
     <row r="233" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B233" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D233" s="13">
         <v>7</v>
@@ -16776,13 +16776,13 @@
     </row>
     <row r="234" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B234" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D234" s="13">
         <v>4</v>
@@ -16840,13 +16840,13 @@
     </row>
     <row r="235" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B235" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D235" s="13">
         <v>36</v>
@@ -16904,13 +16904,13 @@
     </row>
     <row r="236" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B236" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D236" s="13">
         <v>1</v>
@@ -16968,13 +16968,13 @@
     </row>
     <row r="237" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B237" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C237" s="12" t="s">
         <v>314</v>
-      </c>
-      <c r="B237" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C237" s="12" t="s">
-        <v>316</v>
       </c>
       <c r="D237" s="13">
         <v>1</v>
@@ -17032,13 +17032,13 @@
     </row>
     <row r="238" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B238" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D238" s="13">
         <v>2</v>
@@ -17096,13 +17096,13 @@
     </row>
     <row r="239" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B239" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D239" s="13">
         <v>28</v>
@@ -17160,13 +17160,13 @@
     </row>
     <row r="240" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B240" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D240" s="13">
         <v>2</v>
@@ -17224,13 +17224,13 @@
     </row>
     <row r="241" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B241" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="C241" s="12" t="s">
         <v>320</v>
-      </c>
-      <c r="B241" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C241" s="12" t="s">
-        <v>322</v>
       </c>
       <c r="D241" s="13">
         <v>33</v>
@@ -17288,13 +17288,13 @@
     </row>
     <row r="242" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B242" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C242" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D242" s="13">
         <v>9</v>
@@ -17352,13 +17352,13 @@
     </row>
     <row r="243" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B243" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C243" s="12" t="s">
         <v>323</v>
-      </c>
-      <c r="C243" s="12" t="s">
-        <v>325</v>
       </c>
       <c r="D243" s="13">
         <v>27</v>
@@ -17416,13 +17416,13 @@
     </row>
     <row r="244" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B244" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D244" s="13">
         <v>4</v>
@@ -17480,13 +17480,13 @@
     </row>
     <row r="245" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B245" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C245" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D245" s="13">
         <v>2</v>
@@ -17544,13 +17544,13 @@
     </row>
     <row r="246" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B246" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="C246" s="12" t="s">
         <v>327</v>
-      </c>
-      <c r="C246" s="12" t="s">
-        <v>329</v>
       </c>
       <c r="D246" s="13">
         <v>16</v>
@@ -17608,13 +17608,13 @@
     </row>
     <row r="247" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B247" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D247" s="13">
         <v>3</v>
@@ -17670,13 +17670,13 @@
     </row>
     <row r="248" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B248" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D248" s="13">
         <v>12</v>
@@ -17734,13 +17734,13 @@
     </row>
     <row r="249" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B249" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D249" s="13">
         <v>1</v>
@@ -17798,13 +17798,13 @@
     </row>
     <row r="250" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B250" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D250" s="13">
         <v>1</v>
@@ -17862,13 +17862,13 @@
     </row>
     <row r="251" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B251" s="11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D251" s="13">
         <v>2</v>
@@ -17926,13 +17926,13 @@
     </row>
     <row r="252" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B252" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D252" s="13">
         <v>1</v>
@@ -17990,13 +17990,13 @@
     </row>
     <row r="253" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B253" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="C253" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="C253" s="12" t="s">
-        <v>337</v>
       </c>
       <c r="D253" s="13">
         <v>19</v>
@@ -18054,13 +18054,13 @@
     </row>
     <row r="254" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B254" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C254" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D254" s="13">
         <v>6</v>
@@ -18118,13 +18118,13 @@
     </row>
     <row r="255" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D255" s="13">
         <v>1</v>
@@ -18182,13 +18182,13 @@
     </row>
     <row r="256" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B256" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D256" s="13">
         <v>15</v>
@@ -18246,13 +18246,13 @@
     </row>
     <row r="257" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D257" s="13">
         <v>5</v>
@@ -18310,13 +18310,13 @@
     </row>
     <row r="258" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D258" s="13">
         <v>1</v>
@@ -18374,13 +18374,13 @@
     </row>
     <row r="259" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B259" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C259" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D259" s="13">
         <v>7</v>
@@ -18438,13 +18438,13 @@
     </row>
     <row r="260" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C260" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D260" s="13">
         <v>8</v>
@@ -18502,13 +18502,13 @@
     </row>
     <row r="261" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D261" s="13">
         <v>12</v>
@@ -18566,13 +18566,13 @@
     </row>
     <row r="262" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B262" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D262" s="13">
         <v>68</v>
@@ -18630,13 +18630,13 @@
     </row>
     <row r="263" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B263" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D263" s="13">
         <v>4</v>
@@ -18694,13 +18694,13 @@
     </row>
     <row r="264" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B264" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D264" s="13">
         <v>8</v>
@@ -18758,13 +18758,13 @@
     </row>
     <row r="265" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B265" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D265" s="13">
         <v>1</v>
@@ -18822,13 +18822,13 @@
     </row>
     <row r="266" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B266" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C266" s="12" t="s">
         <v>349</v>
-      </c>
-      <c r="B266" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C266" s="12" t="s">
-        <v>351</v>
       </c>
       <c r="D266" s="13">
         <v>6</v>
@@ -18886,13 +18886,13 @@
     </row>
     <row r="267" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B267" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D267" s="13">
         <v>2</v>
@@ -18950,13 +18950,13 @@
     </row>
     <row r="268" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B268" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D268" s="13">
         <v>3</v>
@@ -19012,13 +19012,13 @@
     </row>
     <row r="269" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B269" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D269" s="13">
         <v>1</v>
@@ -19076,13 +19076,13 @@
     </row>
     <row r="270" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B270" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D270" s="13">
         <v>22</v>
@@ -19140,13 +19140,13 @@
     </row>
     <row r="271" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B271" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D271" s="13">
         <v>3</v>
@@ -19202,13 +19202,13 @@
     </row>
     <row r="272" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B272" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C272" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D272" s="13">
         <v>1</v>
@@ -19266,13 +19266,13 @@
     </row>
     <row r="273" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B273" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D273" s="13">
         <v>6</v>
@@ -19330,13 +19330,13 @@
     </row>
     <row r="274" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B274" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D274" s="13">
         <v>2</v>
@@ -19394,13 +19394,13 @@
     </row>
     <row r="275" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B275" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D275" s="13">
         <v>3</v>
@@ -19456,13 +19456,13 @@
     </row>
     <row r="276" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B276" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D276" s="13">
         <v>2</v>
@@ -19520,13 +19520,13 @@
     </row>
     <row r="277" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B277" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D277" s="13">
         <v>3</v>
@@ -19582,13 +19582,13 @@
     </row>
     <row r="278" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B278" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D278" s="13">
         <v>6</v>
@@ -19646,13 +19646,13 @@
     </row>
     <row r="279" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B279" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D279" s="13">
         <v>6</v>
@@ -19710,13 +19710,13 @@
     </row>
     <row r="280" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B280" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D280" s="13">
         <v>2</v>
@@ -19774,13 +19774,13 @@
     </row>
     <row r="281" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B281" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D281" s="13">
         <v>23</v>
@@ -19838,13 +19838,13 @@
     </row>
     <row r="282" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B282" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D282" s="13">
         <v>1</v>
@@ -19902,13 +19902,13 @@
     </row>
     <row r="283" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B283" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D283" s="13">
         <v>1</v>
@@ -19966,13 +19966,13 @@
     </row>
     <row r="284" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B284" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C284" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D284" s="13">
         <v>2</v>
@@ -20030,13 +20030,13 @@
     </row>
     <row r="285" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B285" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D285" s="13">
         <v>2</v>
@@ -20094,13 +20094,13 @@
     </row>
     <row r="286" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B286" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D286" s="13">
         <v>1</v>
@@ -20158,13 +20158,13 @@
     </row>
     <row r="287" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B287" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D287" s="13">
         <v>1</v>
@@ -20222,13 +20222,13 @@
     </row>
     <row r="288" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B288" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D288" s="13">
         <v>1</v>
@@ -20286,13 +20286,13 @@
     </row>
     <row r="289" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B289" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D289" s="13">
         <v>26</v>
@@ -20350,13 +20350,13 @@
     </row>
     <row r="290" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B290" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C290" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D290" s="13">
         <v>5</v>
@@ -20414,13 +20414,13 @@
     </row>
     <row r="291" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B291" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D291" s="13">
         <v>5</v>
@@ -20478,13 +20478,13 @@
     </row>
     <row r="292" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B292" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D292" s="13">
         <v>3</v>
@@ -20540,13 +20540,13 @@
     </row>
     <row r="293" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B293" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D293" s="13">
         <v>2</v>
@@ -20604,13 +20604,13 @@
     </row>
     <row r="294" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B294" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D294" s="13">
         <v>2</v>
@@ -20668,13 +20668,13 @@
     </row>
     <row r="295" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B295" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D295" s="13">
         <v>21</v>
@@ -20732,13 +20732,13 @@
     </row>
     <row r="296" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B296" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D296" s="13">
         <v>6</v>
@@ -20796,13 +20796,13 @@
     </row>
     <row r="297" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B297" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D297" s="13">
         <v>2</v>
@@ -20860,13 +20860,13 @@
     </row>
     <row r="298" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B298" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D298" s="13">
         <v>2</v>
@@ -20924,13 +20924,13 @@
     </row>
     <row r="299" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B299" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D299" s="13">
         <v>6</v>
@@ -20988,13 +20988,13 @@
     </row>
     <row r="300" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="B300" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C300" s="12" t="s">
         <v>383</v>
-      </c>
-      <c r="B300" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C300" s="12" t="s">
-        <v>385</v>
       </c>
       <c r="D300" s="13">
         <v>1</v>
@@ -21052,13 +21052,13 @@
     </row>
     <row r="301" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B301" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D301" s="13">
         <v>1</v>
@@ -21116,13 +21116,13 @@
     </row>
     <row r="302" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B302" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C302" s="12" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D302" s="13">
         <v>4</v>
@@ -21180,13 +21180,13 @@
     </row>
     <row r="303" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B303" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C303" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D303" s="13">
         <v>3</v>
@@ -21242,13 +21242,13 @@
     </row>
     <row r="304" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B304" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C304" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D304" s="13">
         <v>1</v>
@@ -21306,13 +21306,13 @@
     </row>
     <row r="305" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B305" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C305" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D305" s="13">
         <v>1</v>
@@ -21370,13 +21370,13 @@
     </row>
     <row r="306" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B306" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C306" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D306" s="13">
         <v>1</v>
@@ -21434,13 +21434,13 @@
     </row>
     <row r="307" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B307" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C307" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D307" s="13">
         <v>4</v>
@@ -21498,13 +21498,13 @@
     </row>
     <row r="308" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B308" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C308" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D308" s="13">
         <v>2</v>
@@ -21562,13 +21562,13 @@
     </row>
     <row r="309" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B309" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C309" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D309" s="13">
         <v>2</v>
@@ -21626,13 +21626,13 @@
     </row>
     <row r="310" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B310" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C310" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D310" s="13">
         <v>4</v>
@@ -21690,13 +21690,13 @@
     </row>
     <row r="311" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B311" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C311" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D311" s="13">
         <v>1</v>
@@ -21754,13 +21754,13 @@
     </row>
     <row r="312" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B312" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C312" s="12" t="s">
         <v>396</v>
-      </c>
-      <c r="B312" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C312" s="12" t="s">
-        <v>398</v>
       </c>
       <c r="D312" s="13">
         <v>1</v>
@@ -21818,13 +21818,13 @@
     </row>
     <row r="313" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B313" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C313" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D313" s="13">
         <v>1</v>
@@ -21882,13 +21882,13 @@
     </row>
     <row r="314" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B314" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C314" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D314" s="13">
         <v>6</v>
@@ -21946,13 +21946,13 @@
     </row>
     <row r="315" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B315" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C315" s="12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D315" s="13">
         <v>6</v>
@@ -22010,13 +22010,13 @@
     </row>
     <row r="316" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="B316" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C316" s="12" t="s">
         <v>401</v>
-      </c>
-      <c r="B316" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C316" s="12" t="s">
-        <v>403</v>
       </c>
       <c r="D316" s="13">
         <v>1</v>
@@ -22074,13 +22074,13 @@
     </row>
     <row r="317" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B317" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C317" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D317" s="13">
         <v>5</v>
@@ -22138,13 +22138,13 @@
     </row>
     <row r="318" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B318" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C318" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D318" s="13">
         <v>7</v>
@@ -22202,13 +22202,13 @@
     </row>
     <row r="319" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B319" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C319" s="12" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D319" s="13">
         <v>2</v>
@@ -22266,13 +22266,13 @@
     </row>
     <row r="320" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B320" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="C320" s="12" t="s">
         <v>407</v>
-      </c>
-      <c r="C320" s="12" t="s">
-        <v>409</v>
       </c>
       <c r="D320" s="13">
         <v>2</v>
@@ -22330,13 +22330,13 @@
     </row>
     <row r="321" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B321" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C321" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D321" s="13">
         <v>3</v>
@@ -22392,13 +22392,13 @@
     </row>
     <row r="322" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B322" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C322" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D322" s="13">
         <v>18</v>
@@ -22456,13 +22456,13 @@
     </row>
     <row r="323" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B323" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C323" s="12" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D323" s="13">
         <v>1</v>
@@ -22520,13 +22520,13 @@
     </row>
     <row r="324" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B324" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C324" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D324" s="13">
         <v>4</v>

</xml_diff>